<commit_message>
arrumando correção de forma cobrança
</commit_message>
<xml_diff>
--- a/de_para.xlsx
+++ b/de_para.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reclassificação de Cobrança\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400B5666-FB47-4C57-A747-398F92507F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D86A40-AF7E-475B-A6C5-B7A34690AF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{D9E21557-41C3-4609-9599-14711AB60079}"/>
+    <workbookView xWindow="1521" yWindow="1521" windowWidth="16588" windowHeight="8501" xr2:uid="{D9E21557-41C3-4609-9599-14711AB60079}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id_forma_cobranca</t>
   </si>
@@ -87,15 +87,6 @@
   </si>
   <si>
     <t>servico</t>
-  </si>
-  <si>
-    <t>TESTE</t>
-  </si>
-  <si>
-    <t>Gamer</t>
-  </si>
-  <si>
-    <t>All family</t>
   </si>
 </sst>
 </file>
@@ -482,7 +473,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +496,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>196</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -620,31 +611,16 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção e formatação de envio de e-mail
</commit_message>
<xml_diff>
--- a/de_para.xlsx
+++ b/de_para.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reclassificação de Cobrança\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D86A40-AF7E-475B-A6C5-B7A34690AF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597A3BB1-B23F-49E7-AC81-0FAB8E0F1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1521" yWindow="1521" windowWidth="16588" windowHeight="8501" xr2:uid="{D9E21557-41C3-4609-9599-14711AB60079}"/>
+    <workbookView xWindow="22015" yWindow="-104" windowWidth="22325" windowHeight="11924" xr2:uid="{D9E21557-41C3-4609-9599-14711AB60079}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>id_forma_cobranca</t>
   </si>
@@ -50,9 +50,6 @@
     <t>CP NET</t>
   </si>
   <si>
-    <t>C P NET</t>
-  </si>
-  <si>
     <t>CPM</t>
   </si>
   <si>
@@ -87,6 +84,51 @@
   </si>
   <si>
     <t>servico</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALLREDE PARTICIPAÇÕES | Banco do Brasil  </t>
+  </si>
+  <si>
+    <t>BANCO DO BRASIL - CONEX</t>
+  </si>
+  <si>
+    <t>BANCO DO BRASIL - C P NET</t>
+  </si>
+  <si>
+    <t>BANCO DO BRASIL - CPM NET</t>
+  </si>
+  <si>
+    <t>BANCO DO BRASIL - MCP</t>
+  </si>
+  <si>
+    <t>SKILLNET | (EM HOMOLOGAÇÃO NÃO USAR) - CEF-VALPARAISO-SKILL-TELECOM</t>
+  </si>
+  <si>
+    <t>BANCO SICOOB - FLAVIO GARCIA FERREIRA</t>
+  </si>
+  <si>
+    <t>Banco do Brasil | LinkWap</t>
+  </si>
+  <si>
+    <t>LOGTEL | Banco do Brasil TILOG</t>
+  </si>
+  <si>
+    <t>TI5 TELECOM | BB-Link7</t>
+  </si>
+  <si>
+    <t>UNILINK | SICREDI  v2</t>
+  </si>
+  <si>
+    <t>OBTI | CAIXA INTERNO CARTÃO</t>
+  </si>
+  <si>
+    <t>MTEL - BB - 61123-9</t>
+  </si>
+  <si>
+    <t>BANCO DO BRASIL LIGO</t>
   </si>
 </sst>
 </file>
@@ -470,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F79B7D-1A51-4451-A7EB-E1D9B94DB266}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,133 +525,173 @@
     <col min="3" max="3" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>255</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>311</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>304</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
         <v>167</v>
       </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
@@ -617,11 +699,8 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="1"/>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Corrigindo de-para do banco do brasil para bradesco
</commit_message>
<xml_diff>
--- a/de_para.xlsx
+++ b/de_para.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reclassificação de Cobrança\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597A3BB1-B23F-49E7-AC81-0FAB8E0F1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5881C07-9CCE-4281-89D5-5357501943C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22015" yWindow="-104" windowWidth="22325" windowHeight="11924" xr2:uid="{D9E21557-41C3-4609-9599-14711AB60079}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{D9E21557-41C3-4609-9599-14711AB60079}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>descricao</t>
   </si>
   <si>
-    <t xml:space="preserve">ALLREDE PARTICIPAÇÕES | Banco do Brasil  </t>
-  </si>
-  <si>
     <t>BANCO DO BRASIL - CONEX</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>BANCO DO BRASIL LIGO</t>
+  </si>
+  <si>
+    <t>ALLREDE PARTICIPACOES | Bradesco CC</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,10 +541,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>255</v>
+        <v>464</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -555,7 +555,7 @@
         <v>311</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -566,7 +566,7 @@
         <v>304</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -577,7 +577,7 @@
         <v>310</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -588,7 +588,7 @@
         <v>308</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -599,7 +599,7 @@
         <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>395</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -621,7 +621,7 @@
         <v>290</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -632,7 +632,7 @@
         <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
         <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -654,7 +654,7 @@
         <v>251</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -665,7 +665,7 @@
         <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -676,7 +676,7 @@
         <v>365</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -687,7 +687,7 @@
         <v>167</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>